<commit_message>
Keras & Prophet Add_Regressors
Work on Keras and additional Prophet functionality for additional regressors. Updated Prophet demo app and data too.
</commit_message>
<xml_diff>
--- a/docs/VIC-Emergency-Department-Attendances.xlsx
+++ b/docs/VIC-Emergency-Department-Attendances.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17976" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17976" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="45">
   <si>
     <t>Albury Hospital</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE41"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2:AE41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +555,7 @@
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -649,8 +649,26 @@
       <c r="AE1" s="2">
         <v>43617</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF1" s="2">
+        <v>43647</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>43678</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>43709</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>43739</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>43770</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,26 +744,44 @@
       <c r="Y2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -821,26 +857,44 @@
       <c r="Y3" s="8">
         <v>6065</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z3" s="8">
+        <v>6037</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>5592</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>6208</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>5699</v>
+      </c>
+      <c r="AD3" s="8">
+        <v>5886</v>
+      </c>
+      <c r="AE3" s="8">
+        <v>5599</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -916,26 +970,44 @@
       <c r="Y4" s="8">
         <v>3469</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z4" s="8">
+        <v>3323</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>3300</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>3435</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>3383</v>
+      </c>
+      <c r="AD4" s="8">
+        <v>3588</v>
+      </c>
+      <c r="AE4" s="8">
+        <v>3487</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1011,26 +1083,44 @@
       <c r="Y5" s="8">
         <v>7769</v>
       </c>
-      <c r="Z5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z5" s="8">
+        <v>7446</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>7043</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>7934</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>7486</v>
+      </c>
+      <c r="AD5" s="8">
+        <v>7848</v>
+      </c>
+      <c r="AE5" s="8">
+        <v>7642</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1106,26 +1196,44 @@
       <c r="Y6" s="8">
         <v>1937</v>
       </c>
-      <c r="Z6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z6" s="8">
+        <v>1945</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>1511</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>1735</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>1754</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>1741</v>
+      </c>
+      <c r="AE6" s="8">
+        <v>1817</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1201,26 +1309,44 @@
       <c r="Y7" s="8">
         <v>5306</v>
       </c>
-      <c r="Z7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z7" s="8">
+        <v>5251</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>4703</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>5268</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>5033</v>
+      </c>
+      <c r="AD7" s="8">
+        <v>5295</v>
+      </c>
+      <c r="AE7" s="8">
+        <v>5218</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1296,26 +1422,44 @@
       <c r="Y8" s="8">
         <v>1654</v>
       </c>
-      <c r="Z8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z8" s="8">
+        <v>1749</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>1273</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>1464</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>1422</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>1342</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>1374</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1391,26 +1535,44 @@
       <c r="Y9" s="8">
         <v>4681</v>
       </c>
-      <c r="Z9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z9" s="8">
+        <v>4739</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>4505</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>5137</v>
+      </c>
+      <c r="AC9" s="8">
+        <v>4929</v>
+      </c>
+      <c r="AD9" s="8">
+        <v>4970</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>5060</v>
+      </c>
+      <c r="AF9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1486,26 +1648,44 @@
       <c r="Y10" s="8">
         <v>6183</v>
       </c>
-      <c r="Z10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z10" s="8">
+        <v>5880</v>
+      </c>
+      <c r="AA10" s="8">
+        <v>5486</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>6224</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>5710</v>
+      </c>
+      <c r="AD10" s="8">
+        <v>6186</v>
+      </c>
+      <c r="AE10" s="8">
+        <v>5937</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1581,26 +1761,44 @@
       <c r="Y11" s="8">
         <v>5671</v>
       </c>
-      <c r="Z11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z11" s="8">
+        <v>5512</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>5217</v>
+      </c>
+      <c r="AB11" s="8">
+        <v>5789</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>5706</v>
+      </c>
+      <c r="AD11" s="8">
+        <v>6034</v>
+      </c>
+      <c r="AE11" s="8">
+        <v>5858</v>
+      </c>
+      <c r="AF11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1676,26 +1874,44 @@
       <c r="Y12" s="8">
         <v>1558</v>
       </c>
-      <c r="Z12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z12" s="8">
+        <v>1543</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>1287</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>1433</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>1525</v>
+      </c>
+      <c r="AD12" s="8">
+        <v>1476</v>
+      </c>
+      <c r="AE12" s="8">
+        <v>1495</v>
+      </c>
+      <c r="AF12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1771,26 +1987,44 @@
       <c r="Y13" s="8">
         <v>6179</v>
       </c>
-      <c r="Z13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z13" s="8">
+        <v>6116</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>5613</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>6277</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>5740</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>6010</v>
+      </c>
+      <c r="AE13" s="8">
+        <v>5954</v>
+      </c>
+      <c r="AF13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1866,26 +2100,44 @@
       <c r="Y14" s="8">
         <v>2121</v>
       </c>
-      <c r="Z14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z14" s="8">
+        <v>2353</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>1788</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>1963</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>1896</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>1900</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>1868</v>
+      </c>
+      <c r="AF14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1961,26 +2213,44 @@
       <c r="Y15" s="8">
         <v>6857</v>
       </c>
-      <c r="Z15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z15" s="8">
+        <v>6993</v>
+      </c>
+      <c r="AA15" s="8">
+        <v>6403</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>7131</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>6615</v>
+      </c>
+      <c r="AD15" s="8">
+        <v>6944</v>
+      </c>
+      <c r="AE15" s="8">
+        <v>6701</v>
+      </c>
+      <c r="AF15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2056,26 +2326,44 @@
       <c r="Y16" s="1">
         <v>762</v>
       </c>
-      <c r="Z16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z16" s="1">
+        <v>638</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>609</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>708</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>687</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>698</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>627</v>
+      </c>
+      <c r="AF16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2151,26 +2439,44 @@
       <c r="Y17" s="8">
         <v>3639</v>
       </c>
-      <c r="Z17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z17" s="8">
+        <v>3404</v>
+      </c>
+      <c r="AA17" s="8">
+        <v>3249</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>3637</v>
+      </c>
+      <c r="AC17" s="8">
+        <v>3442</v>
+      </c>
+      <c r="AD17" s="8">
+        <v>3554</v>
+      </c>
+      <c r="AE17" s="8">
+        <v>3709</v>
+      </c>
+      <c r="AF17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2246,26 +2552,44 @@
       <c r="Y18" s="8">
         <v>5126</v>
       </c>
-      <c r="Z18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z18" s="8">
+        <v>4852</v>
+      </c>
+      <c r="AA18" s="8">
+        <v>4581</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>5104</v>
+      </c>
+      <c r="AC18" s="8">
+        <v>4770</v>
+      </c>
+      <c r="AD18" s="8">
+        <v>4980</v>
+      </c>
+      <c r="AE18" s="8">
+        <v>4771</v>
+      </c>
+      <c r="AF18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2341,26 +2665,44 @@
       <c r="Y19" s="8">
         <v>1330</v>
       </c>
-      <c r="Z19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z19" s="8">
+        <v>1337</v>
+      </c>
+      <c r="AA19" s="8">
+        <v>1383</v>
+      </c>
+      <c r="AB19" s="8">
+        <v>1524</v>
+      </c>
+      <c r="AC19" s="8">
+        <v>1522</v>
+      </c>
+      <c r="AD19" s="8">
+        <v>1452</v>
+      </c>
+      <c r="AE19" s="8">
+        <v>1468</v>
+      </c>
+      <c r="AF19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK19" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2436,26 +2778,44 @@
       <c r="Y20" s="8">
         <v>3033</v>
       </c>
-      <c r="Z20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE20" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z20" s="8">
+        <v>3045</v>
+      </c>
+      <c r="AA20" s="8">
+        <v>2531</v>
+      </c>
+      <c r="AB20" s="8">
+        <v>2761</v>
+      </c>
+      <c r="AC20" s="8">
+        <v>2708</v>
+      </c>
+      <c r="AD20" s="8">
+        <v>2832</v>
+      </c>
+      <c r="AE20" s="8">
+        <v>2763</v>
+      </c>
+      <c r="AF20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2531,26 +2891,44 @@
       <c r="Y21" s="8">
         <v>7942</v>
       </c>
-      <c r="Z21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z21" s="8">
+        <v>7524</v>
+      </c>
+      <c r="AA21" s="8">
+        <v>7121</v>
+      </c>
+      <c r="AB21" s="8">
+        <v>8227</v>
+      </c>
+      <c r="AC21" s="8">
+        <v>7856</v>
+      </c>
+      <c r="AD21" s="8">
+        <v>8173</v>
+      </c>
+      <c r="AE21" s="8">
+        <v>8260</v>
+      </c>
+      <c r="AF21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2626,26 +3004,44 @@
       <c r="Y22" s="8">
         <v>2329</v>
       </c>
-      <c r="Z22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z22" s="8">
+        <v>2317</v>
+      </c>
+      <c r="AA22" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AB22" s="8">
+        <v>2304</v>
+      </c>
+      <c r="AC22" s="8">
+        <v>2396</v>
+      </c>
+      <c r="AD22" s="8">
+        <v>2099</v>
+      </c>
+      <c r="AE22" s="8">
+        <v>2318</v>
+      </c>
+      <c r="AF22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2721,26 +3117,44 @@
       <c r="Y23" s="8">
         <v>9071</v>
       </c>
-      <c r="Z23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE23" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z23" s="8">
+        <v>8827</v>
+      </c>
+      <c r="AA23" s="8">
+        <v>8348</v>
+      </c>
+      <c r="AB23" s="8">
+        <v>9470</v>
+      </c>
+      <c r="AC23" s="8">
+        <v>8840</v>
+      </c>
+      <c r="AD23" s="8">
+        <v>9405</v>
+      </c>
+      <c r="AE23" s="8">
+        <v>9078</v>
+      </c>
+      <c r="AF23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2816,26 +3230,44 @@
       <c r="Y24" s="8">
         <v>2485</v>
       </c>
-      <c r="Z24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z24" s="8">
+        <v>2707</v>
+      </c>
+      <c r="AA24" s="8">
+        <v>1799</v>
+      </c>
+      <c r="AB24" s="8">
+        <v>2016</v>
+      </c>
+      <c r="AC24" s="8">
+        <v>1943</v>
+      </c>
+      <c r="AD24" s="8">
+        <v>1847</v>
+      </c>
+      <c r="AE24" s="8">
+        <v>1834</v>
+      </c>
+      <c r="AF24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2911,26 +3343,44 @@
       <c r="Y25" s="8">
         <v>6305</v>
       </c>
-      <c r="Z25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z25" s="8">
+        <v>5428</v>
+      </c>
+      <c r="AA25" s="8">
+        <v>6195</v>
+      </c>
+      <c r="AB25" s="8">
+        <v>7024</v>
+      </c>
+      <c r="AC25" s="8">
+        <v>6726</v>
+      </c>
+      <c r="AD25" s="8">
+        <v>7720</v>
+      </c>
+      <c r="AE25" s="8">
+        <v>8024</v>
+      </c>
+      <c r="AF25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3006,26 +3456,44 @@
       <c r="Y26" s="8">
         <v>6895</v>
       </c>
-      <c r="Z26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z26" s="8">
+        <v>6774</v>
+      </c>
+      <c r="AA26" s="8">
+        <v>6248</v>
+      </c>
+      <c r="AB26" s="8">
+        <v>7147</v>
+      </c>
+      <c r="AC26" s="8">
+        <v>6734</v>
+      </c>
+      <c r="AD26" s="8">
+        <v>6725</v>
+      </c>
+      <c r="AE26" s="8">
+        <v>6511</v>
+      </c>
+      <c r="AF26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -3101,26 +3569,44 @@
       <c r="Y27" s="8">
         <v>3871</v>
       </c>
-      <c r="Z27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE27" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z27" s="8">
+        <v>4123</v>
+      </c>
+      <c r="AA27" s="8">
+        <v>3497</v>
+      </c>
+      <c r="AB27" s="8">
+        <v>3792</v>
+      </c>
+      <c r="AC27" s="8">
+        <v>3667</v>
+      </c>
+      <c r="AD27" s="8">
+        <v>3506</v>
+      </c>
+      <c r="AE27" s="8">
+        <v>3484</v>
+      </c>
+      <c r="AF27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3196,26 +3682,44 @@
       <c r="Y28" s="8">
         <v>2191</v>
       </c>
-      <c r="Z28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE28" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z28" s="8">
+        <v>2258</v>
+      </c>
+      <c r="AA28" s="8">
+        <v>2148</v>
+      </c>
+      <c r="AB28" s="8">
+        <v>2294</v>
+      </c>
+      <c r="AC28" s="8">
+        <v>2231</v>
+      </c>
+      <c r="AD28" s="8">
+        <v>2218</v>
+      </c>
+      <c r="AE28" s="8">
+        <v>2160</v>
+      </c>
+      <c r="AF28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -3291,26 +3795,44 @@
       <c r="Y29" s="8">
         <v>2846</v>
       </c>
-      <c r="Z29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE29" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z29" s="8">
+        <v>2769</v>
+      </c>
+      <c r="AA29" s="8">
+        <v>2660</v>
+      </c>
+      <c r="AB29" s="8">
+        <v>2878</v>
+      </c>
+      <c r="AC29" s="8">
+        <v>2769</v>
+      </c>
+      <c r="AD29" s="8">
+        <v>3174</v>
+      </c>
+      <c r="AE29" s="8">
+        <v>2848</v>
+      </c>
+      <c r="AF29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -3386,26 +3908,44 @@
       <c r="Y30" s="8">
         <v>3091</v>
       </c>
-      <c r="Z30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE30" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z30" s="8">
+        <v>2973</v>
+      </c>
+      <c r="AA30" s="8">
+        <v>2819</v>
+      </c>
+      <c r="AB30" s="8">
+        <v>3189</v>
+      </c>
+      <c r="AC30" s="8">
+        <v>2913</v>
+      </c>
+      <c r="AD30" s="8">
+        <v>3148</v>
+      </c>
+      <c r="AE30" s="8">
+        <v>3128</v>
+      </c>
+      <c r="AF30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -3481,26 +4021,44 @@
       <c r="Y31" s="8">
         <v>2264</v>
       </c>
-      <c r="Z31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z31" s="8">
+        <v>2376</v>
+      </c>
+      <c r="AA31" s="8">
+        <v>1897</v>
+      </c>
+      <c r="AB31" s="8">
+        <v>2118</v>
+      </c>
+      <c r="AC31" s="8">
+        <v>2081</v>
+      </c>
+      <c r="AD31" s="8">
+        <v>2136</v>
+      </c>
+      <c r="AE31" s="8">
+        <v>2185</v>
+      </c>
+      <c r="AF31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -3576,26 +4134,44 @@
       <c r="Y32" s="8">
         <v>4384</v>
       </c>
-      <c r="Z32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE32" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z32" s="8">
+        <v>4429</v>
+      </c>
+      <c r="AA32" s="8">
+        <v>4202</v>
+      </c>
+      <c r="AB32" s="8">
+        <v>4635</v>
+      </c>
+      <c r="AC32" s="8">
+        <v>4310</v>
+      </c>
+      <c r="AD32" s="8">
+        <v>4492</v>
+      </c>
+      <c r="AE32" s="8">
+        <v>4303</v>
+      </c>
+      <c r="AF32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -3671,26 +4247,44 @@
       <c r="Y33" s="8">
         <v>7218</v>
       </c>
-      <c r="Z33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z33" s="8">
+        <v>7093</v>
+      </c>
+      <c r="AA33" s="8">
+        <v>6688</v>
+      </c>
+      <c r="AB33" s="8">
+        <v>7478</v>
+      </c>
+      <c r="AC33" s="8">
+        <v>7111</v>
+      </c>
+      <c r="AD33" s="8">
+        <v>7459</v>
+      </c>
+      <c r="AE33" s="8">
+        <v>7504</v>
+      </c>
+      <c r="AF33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK33" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -3766,26 +4360,44 @@
       <c r="Y34" s="8">
         <v>1307</v>
       </c>
-      <c r="Z34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z34" s="8">
+        <v>1252</v>
+      </c>
+      <c r="AA34" s="8">
+        <v>1132</v>
+      </c>
+      <c r="AB34" s="8">
+        <v>1151</v>
+      </c>
+      <c r="AC34" s="8">
+        <v>1188</v>
+      </c>
+      <c r="AD34" s="8">
+        <v>1210</v>
+      </c>
+      <c r="AE34" s="8">
+        <v>1289</v>
+      </c>
+      <c r="AF34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK34" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -3861,26 +4473,44 @@
       <c r="Y35" s="8">
         <v>6821</v>
       </c>
-      <c r="Z35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z35" s="8">
+        <v>6877</v>
+      </c>
+      <c r="AA35" s="8">
+        <v>6056</v>
+      </c>
+      <c r="AB35" s="8">
+        <v>6781</v>
+      </c>
+      <c r="AC35" s="8">
+        <v>6422</v>
+      </c>
+      <c r="AD35" s="8">
+        <v>6559</v>
+      </c>
+      <c r="AE35" s="8">
+        <v>6511</v>
+      </c>
+      <c r="AF35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK35" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -3956,26 +4586,44 @@
       <c r="Y36" s="8">
         <v>4009</v>
       </c>
-      <c r="Z36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE36" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z36" s="8">
+        <v>3860</v>
+      </c>
+      <c r="AA36" s="8">
+        <v>3590</v>
+      </c>
+      <c r="AB36" s="8">
+        <v>3948</v>
+      </c>
+      <c r="AC36" s="8">
+        <v>3846</v>
+      </c>
+      <c r="AD36" s="8">
+        <v>3983</v>
+      </c>
+      <c r="AE36" s="8">
+        <v>3818</v>
+      </c>
+      <c r="AF36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK36" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -4051,26 +4699,44 @@
       <c r="Y37" s="8">
         <v>2123</v>
       </c>
-      <c r="Z37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE37" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z37" s="8">
+        <v>2108</v>
+      </c>
+      <c r="AA37" s="8">
+        <v>1866</v>
+      </c>
+      <c r="AB37" s="8">
+        <v>2009</v>
+      </c>
+      <c r="AC37" s="8">
+        <v>2065</v>
+      </c>
+      <c r="AD37" s="8">
+        <v>2066</v>
+      </c>
+      <c r="AE37" s="8">
+        <v>2116</v>
+      </c>
+      <c r="AF37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK37" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -4146,26 +4812,44 @@
       <c r="Y38" s="8">
         <v>3733</v>
       </c>
-      <c r="Z38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE38" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z38" s="8">
+        <v>3526</v>
+      </c>
+      <c r="AA38" s="8">
+        <v>3273</v>
+      </c>
+      <c r="AB38" s="8">
+        <v>3733</v>
+      </c>
+      <c r="AC38" s="8">
+        <v>3538</v>
+      </c>
+      <c r="AD38" s="8">
+        <v>3547</v>
+      </c>
+      <c r="AE38" s="8">
+        <v>3452</v>
+      </c>
+      <c r="AF38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK38" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -4241,26 +4925,44 @@
       <c r="Y39" s="8">
         <v>1554</v>
       </c>
-      <c r="Z39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z39" s="8">
+        <v>1459</v>
+      </c>
+      <c r="AA39" s="8">
+        <v>1376</v>
+      </c>
+      <c r="AB39" s="8">
+        <v>1384</v>
+      </c>
+      <c r="AC39" s="8">
+        <v>1338</v>
+      </c>
+      <c r="AD39" s="8">
+        <v>1326</v>
+      </c>
+      <c r="AE39" s="8">
+        <v>1225</v>
+      </c>
+      <c r="AF39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -4336,26 +5038,44 @@
       <c r="Y40" s="8">
         <v>1331</v>
       </c>
-      <c r="Z40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE40" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Z40" s="8">
+        <v>1283</v>
+      </c>
+      <c r="AA40" s="8">
+        <v>1056</v>
+      </c>
+      <c r="AB40" s="8">
+        <v>1205</v>
+      </c>
+      <c r="AC40" s="8">
+        <v>1287</v>
+      </c>
+      <c r="AD40" s="8">
+        <v>1314</v>
+      </c>
+      <c r="AE40" s="8">
+        <v>1278</v>
+      </c>
+      <c r="AF40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -4431,22 +5151,40 @@
       <c r="Y41" s="8">
         <v>2735</v>
       </c>
-      <c r="Z41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="5" t="s">
+      <c r="Z41" s="8">
+        <v>2701</v>
+      </c>
+      <c r="AA41" s="8">
+        <v>2464</v>
+      </c>
+      <c r="AB41" s="8">
+        <v>2711</v>
+      </c>
+      <c r="AC41" s="8">
+        <v>2614</v>
+      </c>
+      <c r="AD41" s="8">
+        <v>2635</v>
+      </c>
+      <c r="AE41" s="8">
+        <v>2719</v>
+      </c>
+      <c r="AF41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK41" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4458,10 +5196,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4725,7 +5463,7 @@
         <v>43556</v>
       </c>
       <c r="B29" s="9" t="str">
-        <f t="shared" ref="B29:B31" si="1">"" &amp; _xlfn.NUMBERVALUE(A29)</f>
+        <f t="shared" ref="B29:B32" si="1">"" &amp; _xlfn.NUMBERVALUE(A29)</f>
         <v>43556</v>
       </c>
     </row>
@@ -4745,6 +5483,60 @@
       <c r="B31" s="9" t="str">
         <f t="shared" si="1"/>
         <v>43617</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>43647</v>
+      </c>
+      <c r="B32" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>43678</v>
+      </c>
+      <c r="B33" s="9" t="str">
+        <f t="shared" ref="B33:B37" si="2">"" &amp; _xlfn.NUMBERVALUE(A33)</f>
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>43709</v>
+      </c>
+      <c r="B34" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>43739</v>
+      </c>
+      <c r="B35" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>43770</v>
+      </c>
+      <c r="B36" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>43800</v>
+      </c>
+      <c r="B37" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>